<commit_message>
load to db dataflow
</commit_message>
<xml_diff>
--- a/Timepoints .xlsx
+++ b/Timepoints .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuiThanhDam02GmailGithub\DW_2023_T2_Nhom9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65581216-D153-4BAE-95AF-08CC68A8A473}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2576A18-831B-41BA-90E4-FFBD7346644E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="1428" windowWidth="20520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="1800" windowWidth="20520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>4.1.4 Load warehouse vào datamart</t>
   </si>
   <si>
-    <t>4.1 Dataflow (Workflow)</t>
-  </si>
-  <si>
     <t>4.2.1 Lấy data từ source</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>hoanf thành</t>
   </si>
   <si>
-    <t>4.2 Dataflow (Dataflow)</t>
-  </si>
-  <si>
-    <t>file dataflow sheet extract</t>
-  </si>
-  <si>
     <t>hoàn thành</t>
   </si>
   <si>
@@ -217,6 +208,15 @@
   </si>
   <si>
     <t>file dataflow sheet crawler</t>
+  </si>
+  <si>
+    <t>4.1 Flow (Workflow)</t>
+  </si>
+  <si>
+    <t>4.2 Flow (Dataflow)</t>
+  </si>
+  <si>
+    <t>file dataflow sheet extract, load to staging</t>
   </si>
 </sst>
 </file>
@@ -818,10 +818,10 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
@@ -973,7 +973,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H5" s="27"/>
       <c r="I5" s="35" t="s">
@@ -1245,7 +1245,7 @@
     <row r="17" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="14"/>
       <c r="F17" s="22" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="G17" s="23" t="s">
         <v>31</v>
@@ -1348,7 +1348,7 @@
         <v>51</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="35" t="s">
@@ -1367,7 +1367,7 @@
     <row r="22" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="14"/>
       <c r="F22" s="22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>47</v>
@@ -1383,7 +1383,7 @@
     <row r="23" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="14"/>
       <c r="F23" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="26" t="s">
         <v>6</v>
@@ -1402,7 +1402,7 @@
         <v>45241</v>
       </c>
       <c r="M23" s="43" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N23" s="44" t="s">
         <v>36</v>
@@ -1411,7 +1411,7 @@
     <row r="24" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="14"/>
       <c r="F24" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="26" t="s">
         <v>4</v>
@@ -1430,16 +1430,16 @@
         <v>45088</v>
       </c>
       <c r="M24" s="43" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N24" s="44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="14"/>
       <c r="F25" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>4</v>
@@ -1458,19 +1458,19 @@
         <v>45088</v>
       </c>
       <c r="M25" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="N25" s="44" t="s">
         <v>57</v>
-      </c>
-      <c r="N25" s="44" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="14"/>
       <c r="F26" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="47">

</xml_diff>

<commit_message>
update Plan , Runable file Jar (.bat), fix File
</commit_message>
<xml_diff>
--- a/Timepoints .xlsx
+++ b/Timepoints .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.Student\Nam4_HK1\Data Warehouse\DW_2023_T2_Nhom9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuiThanhDam02GmailGithub\DW_2023_T2_Nhom9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061D124E-49CC-4053-A370-6483E6F168B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D4542-577B-41D6-8ADC-5B0D2DFFF73D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="1236" windowWidth="20520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>Thành Viên</t>
   </si>
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -477,9 +477,6 @@
     <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -504,7 +501,7 @@
     <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -784,28 +781,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="39.5703125" style="26" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" style="26" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="27" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" style="28" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" style="29" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" style="30" customWidth="1"/>
-    <col min="13" max="14" width="30.7109375" style="31" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="23"/>
+    <col min="1" max="1" width="15.109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="39.5546875" style="26" customWidth="1"/>
+    <col min="7" max="8" width="30.6640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="27" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" style="29" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" style="30" customWidth="1"/>
+    <col min="13" max="14" width="30.6640625" style="31" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="25" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="25" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -819,35 +816,35 @@
         <v>7</v>
       </c>
       <c r="E1" s="21"/>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -871,10 +868,10 @@
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-    </row>
-    <row r="3" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+    </row>
+    <row r="3" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -901,11 +898,11 @@
       <c r="M3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
@@ -928,11 +925,11 @@
       <c r="M4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F5" s="11" t="s">
         <v>20</v>
       </c>
@@ -955,11 +952,11 @@
       <c r="M5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
@@ -973,12 +970,18 @@
       <c r="J6" s="33">
         <v>45222</v>
       </c>
-      <c r="K6" s="18"/>
+      <c r="K6" s="34">
+        <v>45229</v>
+      </c>
       <c r="L6" s="11"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
@@ -990,10 +993,10 @@
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-    </row>
-    <row r="8" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+    </row>
+    <row r="8" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F8" s="9" t="s">
         <v>23</v>
       </c>
@@ -1010,11 +1013,11 @@
       <c r="K8" s="18"/>
       <c r="L8" s="11"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="24"/>
       <c r="F9" s="9" t="s">
         <v>24</v>
@@ -1036,7 +1039,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
       <c r="F10" s="9" t="s">
         <v>25</v>
@@ -1058,7 +1061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
       <c r="F11" s="3" t="s">
         <v>52</v>
@@ -1082,11 +1085,11 @@
       <c r="M11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="24"/>
       <c r="F12" s="3" t="s">
         <v>53</v>
@@ -1102,7 +1105,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="24"/>
       <c r="F13" s="9" t="s">
         <v>54</v>
@@ -1126,11 +1129,11 @@
       <c r="M13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="24"/>
       <c r="F14" s="9" t="s">
         <v>55</v>
@@ -1149,16 +1152,16 @@
         <v>45225</v>
       </c>
       <c r="L14" s="34">
-        <v>45229</v>
+        <v>45261</v>
       </c>
       <c r="M14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="N14" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="24"/>
       <c r="F15" s="9" t="s">
         <v>56</v>
@@ -1182,11 +1185,11 @@
       <c r="M15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="24"/>
       <c r="F16" s="9" t="s">
         <v>57</v>
@@ -1210,11 +1213,11 @@
       <c r="M16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="N16" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="24"/>
       <c r="F17" s="9" t="s">
         <v>59</v>
@@ -1238,11 +1241,11 @@
       <c r="M17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N17" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="24"/>
       <c r="F18" s="9" t="s">
         <v>60</v>
@@ -1266,11 +1269,11 @@
       <c r="M18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="N18" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="24"/>
       <c r="F19" s="9" t="s">
         <v>61</v>
@@ -1292,11 +1295,11 @@
         <v>45249</v>
       </c>
       <c r="M19" s="10"/>
-      <c r="N19" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="24"/>
       <c r="F20" s="3" t="s">
         <v>44</v>
@@ -1312,7 +1315,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C21" s="24"/>
       <c r="F21" s="9" t="s">
         <v>34</v>
@@ -1336,11 +1339,11 @@
       <c r="M21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="N21" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C22" s="24"/>
       <c r="F22" s="9" t="s">
         <v>35</v>
@@ -1364,11 +1367,11 @@
       <c r="M22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N22" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C23" s="24"/>
       <c r="F23" s="9" t="s">
         <v>36</v>
@@ -1392,17 +1395,17 @@
       <c r="M23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N23" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C24" s="24"/>
       <c r="F24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="38" t="s">
-        <v>42</v>
+      <c r="G24" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="33">
@@ -1411,12 +1414,18 @@
       <c r="J24" s="34">
         <v>45250</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="11"/>
+      <c r="K24" s="33">
+        <v>45220</v>
+      </c>
+      <c r="L24" s="33">
+        <v>45220</v>
+      </c>
       <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-    </row>
-    <row r="25" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C25" s="24"/>
       <c r="F25" s="3" t="s">
         <v>45</v>
@@ -1432,7 +1441,7 @@
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C26" s="24"/>
       <c r="F26" s="9" t="s">
         <v>38</v>
@@ -1452,17 +1461,17 @@
       <c r="M26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N26" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C27" s="24"/>
       <c r="F27" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="34">
@@ -1476,11 +1485,11 @@
       <c r="M27" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="N27" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C28" s="24"/>
       <c r="F28" s="9" t="s">
         <v>40</v>
@@ -1504,11 +1513,11 @@
       <c r="M28" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N28" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C29" s="24"/>
       <c r="F29" s="9" t="s">
         <v>74</v>
@@ -1532,17 +1541,17 @@
       <c r="M29" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="N29" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C30" s="24"/>
       <c r="F30" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="38" t="s">
-        <v>42</v>
+      <c r="G30" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="34">
@@ -1554,9 +1563,11 @@
       <c r="K30" s="18"/>
       <c r="L30" s="11"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-    </row>
-    <row r="31" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F31" s="9" t="s">
         <v>48</v>
       </c>
@@ -1579,11 +1590,11 @@
       <c r="M31" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="N31" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N31" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F32" s="9" t="s">
         <v>49</v>
       </c>
@@ -1600,17 +1611,17 @@
       <c r="K32" s="16">
         <v>45254</v>
       </c>
-      <c r="L32" s="46">
+      <c r="L32" s="45">
         <v>45256</v>
       </c>
       <c r="M32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="N32" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N32" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F33" s="9" t="s">
         <v>50</v>
       </c>
@@ -1631,11 +1642,11 @@
         <v>45249</v>
       </c>
       <c r="M33" s="10"/>
-      <c r="N33" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N33" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F34" s="9" t="s">
         <v>51</v>
       </c>
@@ -1656,11 +1667,11 @@
         <v>45249</v>
       </c>
       <c r="M34" s="10"/>
-      <c r="N34" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N34" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C35" s="24"/>
       <c r="F35" s="3" t="s">
         <v>65</v>
@@ -1676,7 +1687,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F36" s="9" t="s">
         <v>66</v>
       </c>
@@ -1690,12 +1701,18 @@
       <c r="J36" s="34">
         <v>45255</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="11"/>
+      <c r="K36" s="34">
+        <v>45248</v>
+      </c>
+      <c r="L36" s="34">
+        <v>45248</v>
+      </c>
       <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-    </row>
-    <row r="37" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F37" s="9" t="s">
         <v>67</v>
       </c>
@@ -1716,16 +1733,16 @@
         <v>45248</v>
       </c>
       <c r="M37" s="10"/>
-      <c r="N37" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F38" s="9" t="s">
         <v>68</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="34">
@@ -1741,11 +1758,11 @@
         <v>45248</v>
       </c>
       <c r="M38" s="10"/>
-      <c r="N38" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N38" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F39" s="9" t="s">
         <v>71</v>
       </c>
@@ -1766,11 +1783,11 @@
         <v>45248</v>
       </c>
       <c r="M39" s="10"/>
-      <c r="N39" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N39" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F40" s="9" t="s">
         <v>70</v>
       </c>
@@ -1784,17 +1801,23 @@
       <c r="J40" s="34">
         <v>45255</v>
       </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="11"/>
+      <c r="K40" s="34">
+        <v>45248</v>
+      </c>
+      <c r="L40" s="34">
+        <v>45248</v>
+      </c>
       <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-    </row>
-    <row r="41" spans="3:14" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N40" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F41" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G41" s="38" t="s">
-        <v>42</v>
+      <c r="G41" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="34">
@@ -1803,10 +1826,16 @@
       <c r="J41" s="34">
         <v>45255</v>
       </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="11"/>
+      <c r="K41" s="34">
+        <v>45248</v>
+      </c>
+      <c r="L41" s="34">
+        <v>45248</v>
+      </c>
       <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="N41" s="44" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>